<commit_message>
Added Readme.md and updated requirements.txt
</commit_message>
<xml_diff>
--- a/Searcher/Data/Comparison of Criteria .xlsx
+++ b/Searcher/Data/Comparison of Criteria .xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
-  <workbookPr/>
+  <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Moomookittyclam/Desktop/School work/Fall 2017/Capstone(Project part)/Capstone-Fall-2017/Searcher/Data/"/>
@@ -52,10 +52,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -326,11 +332,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="917641264"/>
-        <c:axId val="917643040"/>
+        <c:axId val="-878428864"/>
+        <c:axId val="-878426544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="917641264"/>
+        <c:axId val="-878428864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -373,7 +379,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="917643040"/>
+        <c:crossAx val="-878426544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -381,7 +387,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="917643040"/>
+        <c:axId val="-878426544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -432,7 +438,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="917641264"/>
+        <c:crossAx val="-878428864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1115,16 +1121,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1463,8 +1469,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>